<commit_message>
UnitChef successfully applies parameters in the right places. Changed UnitChef._link_area() routine to use plain vanilla link (that starts with `=`) and auto-typing, but dates still show up as integers. Moving on to LineChef for now, to check how financials spreading works.
</commit_message>
<xml_diff>
--- a/blackbird_engine/core/books/m4.xlsx
+++ b/blackbird_engine/core/books/m4.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\blackbird\Engine\mechanics\spread_em\blackbird_engine\core\books\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" activeTab="3"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Scenarios" sheetId="2" r:id="rId2"/>
-    <sheet name="Timeline" sheetId="3" r:id="rId3"/>
-    <sheet name="ef71ceab" sheetId="4" r:id="rId4"/>
-  </sheets>
-  <calcPr calcId="152511"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Scenarios" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Timeline" sheetId="3" r:id="rId3"/>
+    <s:sheet name="ef71ceab" sheetId="4" r:id="rId4"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>annual_inflation</t>
   </si>
@@ -54,22 +49,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,25 +80,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -391,2464 +378,2486 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
         <f>E1</f>
+        <v/>
+      </c>
+      <c r="E1" t="n">
         <v>0.03</v>
       </c>
-      <c r="E1">
-        <v>0.03</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
         <f>E2</f>
+        <v/>
+      </c>
+      <c r="E2" t="n">
         <v>8080</v>
       </c>
-      <c r="E2">
-        <v>8080</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
         <f>E3</f>
-        <v>453.2</v>
-      </c>
-      <c r="E3">
+        <v/>
+      </c>
+      <c r="E3" t="n">
         <v>453.2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A3:BY6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="E3" s="1">
+    <row r="3" spans="1:77">
+      <c r="E3" s="1" t="n">
         <v>41090</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="1" t="n">
         <v>41121</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1" t="n">
         <v>41152</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1" t="n">
         <v>41182</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="1" t="n">
         <v>41213</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="1" t="n">
         <v>41243</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="1" t="n">
         <v>41274</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="1" t="n">
         <v>41305</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="1" t="n">
         <v>41333</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="1" t="n">
         <v>41364</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="1" t="n">
         <v>41394</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="1" t="n">
         <v>41425</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="Q3" s="1" t="n">
         <v>41455</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="1" t="n">
         <v>41486</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="1" t="n">
         <v>41517</v>
       </c>
-      <c r="T3" s="1">
+      <c r="T3" s="1" t="n">
         <v>41547</v>
       </c>
-      <c r="U3" s="1">
+      <c r="U3" s="1" t="n">
         <v>41578</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="1" t="n">
         <v>41608</v>
       </c>
-      <c r="W3" s="1">
+      <c r="W3" s="1" t="n">
         <v>41639</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3" s="1" t="n">
         <v>41670</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Y3" s="1" t="n">
         <v>41698</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="Z3" s="1" t="n">
         <v>41729</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AA3" s="1" t="n">
         <v>41759</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3" s="1" t="n">
         <v>41790</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AC3" s="1" t="n">
         <v>41820</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AD3" s="1" t="n">
         <v>41851</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AE3" s="1" t="n">
         <v>41882</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AF3" s="1" t="n">
         <v>41912</v>
       </c>
-      <c r="AG3" s="1">
+      <c r="AG3" s="1" t="n">
         <v>41943</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AH3" s="1" t="n">
         <v>41973</v>
       </c>
-      <c r="AI3" s="1">
+      <c r="AI3" s="1" t="n">
         <v>42004</v>
       </c>
-      <c r="AJ3" s="1">
+      <c r="AJ3" s="1" t="n">
         <v>42035</v>
       </c>
-      <c r="AK3" s="1">
+      <c r="AK3" s="1" t="n">
         <v>42063</v>
       </c>
-      <c r="AL3" s="1">
+      <c r="AL3" s="1" t="n">
         <v>42094</v>
       </c>
-      <c r="AM3" s="1">
+      <c r="AM3" s="1" t="n">
         <v>42124</v>
       </c>
-      <c r="AN3" s="1">
+      <c r="AN3" s="1" t="n">
         <v>42155</v>
       </c>
-      <c r="AO3" s="1">
+      <c r="AO3" s="1" t="n">
         <v>42185</v>
       </c>
-      <c r="AP3" s="1">
+      <c r="AP3" s="1" t="n">
         <v>42216</v>
       </c>
-      <c r="AQ3" s="1">
+      <c r="AQ3" s="1" t="n">
         <v>42247</v>
       </c>
-      <c r="AR3" s="1">
+      <c r="AR3" s="1" t="n">
         <v>42277</v>
       </c>
-      <c r="AS3" s="1">
+      <c r="AS3" s="1" t="n">
         <v>42308</v>
       </c>
-      <c r="AT3" s="1">
+      <c r="AT3" s="1" t="n">
         <v>42338</v>
       </c>
-      <c r="AU3" s="1">
+      <c r="AU3" s="1" t="n">
         <v>42369</v>
       </c>
-      <c r="AV3" s="1">
+      <c r="AV3" s="1" t="n">
         <v>42400</v>
       </c>
-      <c r="AW3" s="1">
+      <c r="AW3" s="1" t="n">
         <v>42429</v>
       </c>
-      <c r="AX3" s="1">
+      <c r="AX3" s="1" t="n">
         <v>42460</v>
       </c>
-      <c r="AY3" s="1">
+      <c r="AY3" s="1" t="n">
         <v>42490</v>
       </c>
-      <c r="AZ3" s="1">
+      <c r="AZ3" s="1" t="n">
         <v>42521</v>
       </c>
-      <c r="BA3" s="1">
+      <c r="BA3" s="1" t="n">
         <v>42551</v>
       </c>
-      <c r="BB3" s="1">
+      <c r="BB3" s="1" t="n">
         <v>42582</v>
       </c>
-      <c r="BC3" s="1">
+      <c r="BC3" s="1" t="n">
         <v>42613</v>
       </c>
-      <c r="BD3" s="1">
+      <c r="BD3" s="1" t="n">
         <v>42643</v>
       </c>
-      <c r="BE3" s="1">
+      <c r="BE3" s="1" t="n">
         <v>42674</v>
       </c>
-      <c r="BF3" s="1">
+      <c r="BF3" s="1" t="n">
         <v>42704</v>
       </c>
-      <c r="BG3" s="1">
+      <c r="BG3" s="1" t="n">
         <v>42735</v>
       </c>
-      <c r="BH3" s="1">
+      <c r="BH3" s="1" t="n">
         <v>42766</v>
       </c>
-      <c r="BI3" s="1">
+      <c r="BI3" s="1" t="n">
         <v>42794</v>
       </c>
-      <c r="BJ3" s="1">
+      <c r="BJ3" s="1" t="n">
         <v>42825</v>
       </c>
-      <c r="BK3" s="1">
+      <c r="BK3" s="1" t="n">
         <v>42855</v>
       </c>
-      <c r="BL3" s="1">
+      <c r="BL3" s="1" t="n">
         <v>42886</v>
       </c>
-      <c r="BM3" s="1">
+      <c r="BM3" s="1" t="n">
         <v>42916</v>
       </c>
-      <c r="BN3" s="1">
+      <c r="BN3" s="1" t="n">
         <v>42947</v>
       </c>
-      <c r="BO3" s="1">
+      <c r="BO3" s="1" t="n">
         <v>42978</v>
       </c>
-      <c r="BP3" s="1">
+      <c r="BP3" s="1" t="n">
         <v>43008</v>
       </c>
-      <c r="BQ3" s="1">
+      <c r="BQ3" s="1" t="n">
         <v>43039</v>
       </c>
-      <c r="BR3" s="1">
+      <c r="BR3" s="1" t="n">
         <v>43069</v>
       </c>
-      <c r="BS3" s="1">
+      <c r="BS3" s="1" t="n">
         <v>43100</v>
       </c>
-      <c r="BT3" s="1">
+      <c r="BT3" s="1" t="n">
         <v>43131</v>
       </c>
-      <c r="BU3" s="1">
+      <c r="BU3" s="1" t="n">
         <v>43159</v>
       </c>
-      <c r="BV3" s="1">
+      <c r="BV3" s="1" t="n">
         <v>43190</v>
       </c>
-      <c r="BW3" s="1">
+      <c r="BW3" s="1" t="n">
         <v>43220</v>
       </c>
-      <c r="BX3" s="1">
+      <c r="BX3" s="1" t="n">
         <v>43251</v>
       </c>
-      <c r="BY3" s="1">
+      <c r="BY3" s="1" t="n">
         <v>43281</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+    <row r="4" spans="1:77">
+      <c r="A4">
         <f>Scenarios!A1</f>
-        <v>annual_inflation</v>
+        <v/>
       </c>
       <c r="C4">
         <f>Scenarios!C1</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="E4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="F4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="G4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="H4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="I4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="J4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="K4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="L4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="M4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="N4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="O4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="P4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="Q4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="R4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="S4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="T4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="U4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="V4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="W4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="X4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="Y4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="Z4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AA4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AB4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AC4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AD4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AE4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AF4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AG4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AH4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AI4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AJ4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AK4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AL4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AM4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AN4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AO4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AP4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AQ4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AR4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AS4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AT4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AU4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AV4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AW4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AX4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AY4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AZ4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BA4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BB4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BC4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BD4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BE4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BF4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BG4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BH4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BI4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BJ4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BK4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BL4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BM4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BN4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BO4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BP4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BQ4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BR4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BS4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BT4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BU4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BV4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BW4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BX4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BY4">
         <f>C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
+    <row r="5" spans="1:77">
+      <c r="A5">
         <f>Scenarios!A2</f>
-        <v>ltm ga</v>
+        <v/>
       </c>
       <c r="C5">
         <f>Scenarios!C2</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="E5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="F5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="G5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="H5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="I5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="J5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="K5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="L5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="M5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="N5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="O5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="P5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="Q5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="R5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="S5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="T5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="U5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="V5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="W5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="X5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="Y5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="Z5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AA5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AB5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AC5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AD5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AE5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AF5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AG5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AH5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AI5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AJ5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AK5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AL5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AM5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AN5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AO5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AP5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AQ5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AR5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AS5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AT5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AU5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AV5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AW5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AX5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AY5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AZ5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BA5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BB5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BC5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BD5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BE5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BF5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BG5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BH5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BI5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BJ5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BK5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BL5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BM5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BN5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BO5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BP5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BQ5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BR5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BS5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BT5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BU5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BV5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BW5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BX5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BY5">
         <f>C5</f>
-        <v>8080</v>
+        <v/>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+    <row r="6" spans="1:77">
+      <c r="A6">
         <f>Scenarios!A3</f>
-        <v>ltm marketing</v>
+        <v/>
       </c>
       <c r="C6">
         <f>Scenarios!C3</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="E6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="F6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="G6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="H6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="I6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="J6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="K6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="L6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="M6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="N6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="O6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="P6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="Q6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="R6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="S6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="T6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="U6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="V6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="W6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="X6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="Y6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="Z6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AA6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AB6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AC6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AD6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AE6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AF6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AG6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AH6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AI6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AJ6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AK6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AL6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AM6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AN6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AO6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AP6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AQ6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AR6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AS6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AT6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AU6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AV6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AW6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AX6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AY6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AZ6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BA6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BB6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BC6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BD6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BE6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BF6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BG6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BH6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BI6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BJ6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BK6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BL6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BM6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BN6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BO6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BP6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BQ6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BR6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BS6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BT6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BU6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BV6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BW6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BX6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BY6">
         <f>C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A3:BY10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AO10" sqref="AO10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77">
       <c r="E3">
         <f>Timeline!E3</f>
-        <v>41090</v>
+        <v/>
       </c>
       <c r="F3">
         <f>Timeline!F3</f>
-        <v>41121</v>
+        <v/>
       </c>
       <c r="G3">
         <f>Timeline!G3</f>
-        <v>41152</v>
+        <v/>
       </c>
       <c r="H3">
         <f>Timeline!H3</f>
-        <v>41182</v>
+        <v/>
       </c>
       <c r="I3">
         <f>Timeline!I3</f>
-        <v>41213</v>
+        <v/>
       </c>
       <c r="J3">
         <f>Timeline!J3</f>
-        <v>41243</v>
+        <v/>
       </c>
       <c r="K3">
         <f>Timeline!K3</f>
-        <v>41274</v>
+        <v/>
       </c>
       <c r="L3">
         <f>Timeline!L3</f>
-        <v>41305</v>
+        <v/>
       </c>
       <c r="M3">
         <f>Timeline!M3</f>
-        <v>41333</v>
+        <v/>
       </c>
       <c r="N3">
         <f>Timeline!N3</f>
-        <v>41364</v>
+        <v/>
       </c>
       <c r="O3">
         <f>Timeline!O3</f>
-        <v>41394</v>
+        <v/>
       </c>
       <c r="P3">
         <f>Timeline!P3</f>
-        <v>41425</v>
+        <v/>
       </c>
       <c r="Q3">
         <f>Timeline!Q3</f>
-        <v>41455</v>
+        <v/>
       </c>
       <c r="R3">
         <f>Timeline!R3</f>
-        <v>41486</v>
+        <v/>
       </c>
       <c r="S3">
         <f>Timeline!S3</f>
-        <v>41517</v>
+        <v/>
       </c>
       <c r="T3">
         <f>Timeline!T3</f>
-        <v>41547</v>
+        <v/>
       </c>
       <c r="U3">
         <f>Timeline!U3</f>
-        <v>41578</v>
+        <v/>
       </c>
       <c r="V3">
         <f>Timeline!V3</f>
-        <v>41608</v>
+        <v/>
       </c>
       <c r="W3">
         <f>Timeline!W3</f>
-        <v>41639</v>
+        <v/>
       </c>
       <c r="X3">
         <f>Timeline!X3</f>
-        <v>41670</v>
+        <v/>
       </c>
       <c r="Y3">
         <f>Timeline!Y3</f>
-        <v>41698</v>
+        <v/>
       </c>
       <c r="Z3">
         <f>Timeline!Z3</f>
-        <v>41729</v>
+        <v/>
       </c>
       <c r="AA3">
         <f>Timeline!AA3</f>
-        <v>41759</v>
+        <v/>
       </c>
       <c r="AB3">
         <f>Timeline!AB3</f>
-        <v>41790</v>
+        <v/>
       </c>
       <c r="AC3">
         <f>Timeline!AC3</f>
-        <v>41820</v>
+        <v/>
       </c>
       <c r="AD3">
         <f>Timeline!AD3</f>
-        <v>41851</v>
+        <v/>
       </c>
       <c r="AE3">
         <f>Timeline!AE3</f>
-        <v>41882</v>
+        <v/>
       </c>
       <c r="AF3">
         <f>Timeline!AF3</f>
-        <v>41912</v>
+        <v/>
       </c>
       <c r="AG3">
         <f>Timeline!AG3</f>
-        <v>41943</v>
+        <v/>
       </c>
       <c r="AH3">
         <f>Timeline!AH3</f>
-        <v>41973</v>
+        <v/>
       </c>
       <c r="AI3">
         <f>Timeline!AI3</f>
-        <v>42004</v>
+        <v/>
       </c>
       <c r="AJ3">
         <f>Timeline!AJ3</f>
-        <v>42035</v>
+        <v/>
       </c>
       <c r="AK3">
         <f>Timeline!AK3</f>
-        <v>42063</v>
+        <v/>
       </c>
       <c r="AL3">
         <f>Timeline!AL3</f>
-        <v>42094</v>
+        <v/>
       </c>
       <c r="AM3">
         <f>Timeline!AM3</f>
-        <v>42124</v>
+        <v/>
       </c>
       <c r="AN3">
         <f>Timeline!AN3</f>
-        <v>42155</v>
+        <v/>
       </c>
       <c r="AO3">
         <f>Timeline!AO3</f>
-        <v>42185</v>
+        <v/>
       </c>
       <c r="AP3">
         <f>Timeline!AP3</f>
-        <v>42216</v>
+        <v/>
       </c>
       <c r="AQ3">
         <f>Timeline!AQ3</f>
-        <v>42247</v>
+        <v/>
       </c>
       <c r="AR3">
         <f>Timeline!AR3</f>
-        <v>42277</v>
+        <v/>
       </c>
       <c r="AS3">
         <f>Timeline!AS3</f>
-        <v>42308</v>
+        <v/>
       </c>
       <c r="AT3">
         <f>Timeline!AT3</f>
-        <v>42338</v>
+        <v/>
       </c>
       <c r="AU3">
         <f>Timeline!AU3</f>
-        <v>42369</v>
+        <v/>
       </c>
       <c r="AV3">
         <f>Timeline!AV3</f>
-        <v>42400</v>
+        <v/>
       </c>
       <c r="AW3">
         <f>Timeline!AW3</f>
-        <v>42429</v>
+        <v/>
       </c>
       <c r="AX3">
         <f>Timeline!AX3</f>
-        <v>42460</v>
+        <v/>
       </c>
       <c r="AY3">
         <f>Timeline!AY3</f>
-        <v>42490</v>
+        <v/>
       </c>
       <c r="AZ3">
         <f>Timeline!AZ3</f>
-        <v>42521</v>
+        <v/>
       </c>
       <c r="BA3">
         <f>Timeline!BA3</f>
-        <v>42551</v>
+        <v/>
       </c>
       <c r="BB3">
         <f>Timeline!BB3</f>
-        <v>42582</v>
+        <v/>
       </c>
       <c r="BC3">
         <f>Timeline!BC3</f>
-        <v>42613</v>
+        <v/>
       </c>
       <c r="BD3">
         <f>Timeline!BD3</f>
-        <v>42643</v>
+        <v/>
       </c>
       <c r="BE3">
         <f>Timeline!BE3</f>
-        <v>42674</v>
+        <v/>
       </c>
       <c r="BF3">
         <f>Timeline!BF3</f>
-        <v>42704</v>
+        <v/>
       </c>
       <c r="BG3">
         <f>Timeline!BG3</f>
-        <v>42735</v>
+        <v/>
       </c>
       <c r="BH3">
         <f>Timeline!BH3</f>
-        <v>42766</v>
+        <v/>
       </c>
       <c r="BI3">
         <f>Timeline!BI3</f>
-        <v>42794</v>
+        <v/>
       </c>
       <c r="BJ3">
         <f>Timeline!BJ3</f>
-        <v>42825</v>
+        <v/>
       </c>
       <c r="BK3">
         <f>Timeline!BK3</f>
-        <v>42855</v>
+        <v/>
       </c>
       <c r="BL3">
         <f>Timeline!BL3</f>
-        <v>42886</v>
+        <v/>
       </c>
       <c r="BM3">
         <f>Timeline!BM3</f>
-        <v>42916</v>
+        <v/>
       </c>
       <c r="BN3">
         <f>Timeline!BN3</f>
-        <v>42947</v>
+        <v/>
       </c>
       <c r="BO3">
         <f>Timeline!BO3</f>
-        <v>42978</v>
+        <v/>
       </c>
       <c r="BP3">
         <f>Timeline!BP3</f>
-        <v>43008</v>
+        <v/>
       </c>
       <c r="BQ3">
         <f>Timeline!BQ3</f>
-        <v>43039</v>
+        <v/>
       </c>
       <c r="BR3">
         <f>Timeline!BR3</f>
-        <v>43069</v>
+        <v/>
       </c>
       <c r="BS3">
         <f>Timeline!BS3</f>
-        <v>43100</v>
+        <v/>
       </c>
       <c r="BT3">
         <f>Timeline!BT3</f>
-        <v>43131</v>
+        <v/>
       </c>
       <c r="BU3">
         <f>Timeline!BU3</f>
-        <v>43159</v>
+        <v/>
       </c>
       <c r="BV3">
         <f>Timeline!BV3</f>
-        <v>43190</v>
+        <v/>
       </c>
       <c r="BW3">
         <f>Timeline!BW3</f>
-        <v>43220</v>
+        <v/>
       </c>
       <c r="BX3">
         <f>Timeline!BX3</f>
-        <v>43251</v>
+        <v/>
       </c>
       <c r="BY3">
         <f>Timeline!BY3</f>
-        <v>43281</v>
+        <v/>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+    <row r="4" spans="1:77">
+      <c r="A4">
         <f>Timeline!A4</f>
-        <v>annual_inflation</v>
+        <v/>
       </c>
       <c r="C4">
         <f>Timeline!C4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="E4">
         <f>Timeline!E4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="F4">
         <f>Timeline!F4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="G4">
         <f>Timeline!G4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="H4">
         <f>Timeline!H4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="I4">
         <f>Timeline!I4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="J4">
         <f>Timeline!J4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="K4">
         <f>Timeline!K4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="L4">
         <f>Timeline!L4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="M4">
         <f>Timeline!M4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="N4">
         <f>Timeline!N4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="O4">
         <f>Timeline!O4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="P4">
         <f>Timeline!P4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="Q4">
         <f>Timeline!Q4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="R4">
         <f>Timeline!R4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="S4">
         <f>Timeline!S4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="T4">
         <f>Timeline!T4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="U4">
         <f>Timeline!U4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="V4">
         <f>Timeline!V4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="W4">
         <f>Timeline!W4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="X4">
         <f>Timeline!X4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="Y4">
         <f>Timeline!Y4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="Z4">
         <f>Timeline!Z4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AA4">
         <f>Timeline!AA4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AB4">
         <f>Timeline!AB4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AC4">
         <f>Timeline!AC4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AD4">
         <f>Timeline!AD4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AE4">
         <f>Timeline!AE4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AF4">
         <f>Timeline!AF4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AG4">
         <f>Timeline!AG4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AH4">
         <f>Timeline!AH4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AI4">
         <f>Timeline!AI4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AJ4">
         <f>Timeline!AJ4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AK4">
         <f>Timeline!AK4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AL4">
         <f>Timeline!AL4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AM4">
         <f>Timeline!AM4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AN4">
         <f>Timeline!AN4</f>
-        <v>0.03</v>
-      </c>
-      <c r="AO4">
+        <v/>
+      </c>
+      <c r="AO4" t="n">
         <v>0.01</v>
       </c>
       <c r="AP4">
         <f>Timeline!AP4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AQ4">
         <f>Timeline!AQ4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AR4">
         <f>Timeline!AR4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AS4">
         <f>Timeline!AS4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AT4">
         <f>Timeline!AT4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AU4">
         <f>Timeline!AU4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AV4">
         <f>Timeline!AV4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AW4">
         <f>Timeline!AW4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AX4">
         <f>Timeline!AX4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AY4">
         <f>Timeline!AY4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="AZ4">
         <f>Timeline!AZ4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BA4">
         <f>Timeline!BA4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BB4">
         <f>Timeline!BB4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BC4">
         <f>Timeline!BC4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BD4">
         <f>Timeline!BD4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BE4">
         <f>Timeline!BE4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BF4">
         <f>Timeline!BF4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BG4">
         <f>Timeline!BG4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BH4">
         <f>Timeline!BH4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BI4">
         <f>Timeline!BI4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BJ4">
         <f>Timeline!BJ4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BK4">
         <f>Timeline!BK4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BL4">
         <f>Timeline!BL4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BM4">
         <f>Timeline!BM4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BN4">
         <f>Timeline!BN4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BO4">
         <f>Timeline!BO4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BP4">
         <f>Timeline!BP4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BQ4">
         <f>Timeline!BQ4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BR4">
         <f>Timeline!BR4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BS4">
         <f>Timeline!BS4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BT4">
         <f>Timeline!BT4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BU4">
         <f>Timeline!BU4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BV4">
         <f>Timeline!BV4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BW4">
         <f>Timeline!BW4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BX4">
         <f>Timeline!BX4</f>
-        <v>0.03</v>
+        <v/>
       </c>
       <c r="BY4">
         <f>Timeline!BY4</f>
-        <v>0.03</v>
+        <v/>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
+    <row r="5" spans="1:77">
+      <c r="A5">
         <f>Timeline!A5</f>
-        <v>ltm ga</v>
+        <v/>
       </c>
       <c r="C5">
         <f>Timeline!C5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="E5">
         <f>Timeline!E5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="F5">
         <f>Timeline!F5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="G5">
         <f>Timeline!G5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="H5">
         <f>Timeline!H5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="I5">
         <f>Timeline!I5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="J5">
         <f>Timeline!J5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="K5">
         <f>Timeline!K5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="L5">
         <f>Timeline!L5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="M5">
         <f>Timeline!M5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="N5">
         <f>Timeline!N5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="O5">
         <f>Timeline!O5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="P5">
         <f>Timeline!P5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="Q5">
         <f>Timeline!Q5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="R5">
         <f>Timeline!R5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="S5">
         <f>Timeline!S5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="T5">
         <f>Timeline!T5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="U5">
         <f>Timeline!U5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="V5">
         <f>Timeline!V5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="W5">
         <f>Timeline!W5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="X5">
         <f>Timeline!X5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="Y5">
         <f>Timeline!Y5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="Z5">
         <f>Timeline!Z5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AA5">
         <f>Timeline!AA5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AB5">
         <f>Timeline!AB5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AC5">
         <f>Timeline!AC5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AD5">
         <f>Timeline!AD5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AE5">
         <f>Timeline!AE5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AF5">
         <f>Timeline!AF5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AG5">
         <f>Timeline!AG5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AH5">
         <f>Timeline!AH5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AI5">
         <f>Timeline!AI5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AJ5">
         <f>Timeline!AJ5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AK5">
         <f>Timeline!AK5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AL5">
         <f>Timeline!AL5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AM5">
         <f>Timeline!AM5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AN5">
         <f>Timeline!AN5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AO5">
         <f>Timeline!AO5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AP5">
         <f>Timeline!AP5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AQ5">
         <f>Timeline!AQ5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AR5">
         <f>Timeline!AR5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AS5">
         <f>Timeline!AS5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AT5">
         <f>Timeline!AT5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AU5">
         <f>Timeline!AU5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AV5">
         <f>Timeline!AV5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AW5">
         <f>Timeline!AW5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AX5">
         <f>Timeline!AX5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AY5">
         <f>Timeline!AY5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="AZ5">
         <f>Timeline!AZ5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BA5">
         <f>Timeline!BA5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BB5">
         <f>Timeline!BB5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BC5">
         <f>Timeline!BC5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BD5">
         <f>Timeline!BD5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BE5">
         <f>Timeline!BE5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BF5">
         <f>Timeline!BF5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BG5">
         <f>Timeline!BG5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BH5">
         <f>Timeline!BH5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BI5">
         <f>Timeline!BI5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BJ5">
         <f>Timeline!BJ5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BK5">
         <f>Timeline!BK5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BL5">
         <f>Timeline!BL5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BM5">
         <f>Timeline!BM5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BN5">
         <f>Timeline!BN5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BO5">
         <f>Timeline!BO5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BP5">
         <f>Timeline!BP5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BQ5">
         <f>Timeline!BQ5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BR5">
         <f>Timeline!BR5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BS5">
         <f>Timeline!BS5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BT5">
         <f>Timeline!BT5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BU5">
         <f>Timeline!BU5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BV5">
         <f>Timeline!BV5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BW5">
         <f>Timeline!BW5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BX5">
         <f>Timeline!BX5</f>
-        <v>8080</v>
+        <v/>
       </c>
       <c r="BY5">
         <f>Timeline!BY5</f>
-        <v>8080</v>
+        <v/>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+    <row r="6" spans="1:77">
+      <c r="A6">
         <f>Timeline!A6</f>
-        <v>ltm marketing</v>
+        <v/>
       </c>
       <c r="C6">
         <f>Timeline!C6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="E6">
         <f>Timeline!E6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="F6">
         <f>Timeline!F6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="G6">
         <f>Timeline!G6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="H6">
         <f>Timeline!H6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="I6">
         <f>Timeline!I6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="J6">
         <f>Timeline!J6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="K6">
         <f>Timeline!K6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="L6">
         <f>Timeline!L6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="M6">
         <f>Timeline!M6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="N6">
         <f>Timeline!N6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="O6">
         <f>Timeline!O6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="P6">
         <f>Timeline!P6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="Q6">
         <f>Timeline!Q6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="R6">
         <f>Timeline!R6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="S6">
         <f>Timeline!S6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="T6">
         <f>Timeline!T6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="U6">
         <f>Timeline!U6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="V6">
         <f>Timeline!V6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="W6">
         <f>Timeline!W6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="X6">
         <f>Timeline!X6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="Y6">
         <f>Timeline!Y6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="Z6">
         <f>Timeline!Z6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AA6">
         <f>Timeline!AA6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AB6">
         <f>Timeline!AB6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AC6">
         <f>Timeline!AC6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AD6">
         <f>Timeline!AD6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AE6">
         <f>Timeline!AE6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AF6">
         <f>Timeline!AF6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AG6">
         <f>Timeline!AG6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AH6">
         <f>Timeline!AH6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AI6">
         <f>Timeline!AI6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AJ6">
         <f>Timeline!AJ6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AK6">
         <f>Timeline!AK6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AL6">
         <f>Timeline!AL6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AM6">
         <f>Timeline!AM6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AN6">
         <f>Timeline!AN6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AO6">
         <f>Timeline!AO6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AP6">
         <f>Timeline!AP6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AQ6">
         <f>Timeline!AQ6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AR6">
         <f>Timeline!AR6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AS6">
         <f>Timeline!AS6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AT6">
         <f>Timeline!AT6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AU6">
         <f>Timeline!AU6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AV6">
         <f>Timeline!AV6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AW6">
         <f>Timeline!AW6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AX6">
         <f>Timeline!AX6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AY6">
         <f>Timeline!AY6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="AZ6">
         <f>Timeline!AZ6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BA6">
         <f>Timeline!BA6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BB6">
         <f>Timeline!BB6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BC6">
         <f>Timeline!BC6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BD6">
         <f>Timeline!BD6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BE6">
         <f>Timeline!BE6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BF6">
         <f>Timeline!BF6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BG6">
         <f>Timeline!BG6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BH6">
         <f>Timeline!BH6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BI6">
         <f>Timeline!BI6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BJ6">
         <f>Timeline!BJ6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BK6">
         <f>Timeline!BK6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BL6">
         <f>Timeline!BL6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BM6">
         <f>Timeline!BM6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BN6">
         <f>Timeline!BN6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BO6">
         <f>Timeline!BO6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BP6">
         <f>Timeline!BP6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BQ6">
         <f>Timeline!BQ6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BR6">
         <f>Timeline!BR6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BS6">
         <f>Timeline!BS6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BT6">
         <f>Timeline!BT6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BU6">
         <f>Timeline!BU6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BV6">
         <f>Timeline!BV6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BW6">
         <f>Timeline!BW6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BX6">
         <f>Timeline!BX6</f>
-        <v>453.2</v>
+        <v/>
       </c>
       <c r="BY6">
         <f>Timeline!BY6</f>
-        <v>453.2</v>
+        <v/>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>2407</v>
       </c>
       <c r="AO7">
         <f>C7</f>
-        <v>2407</v>
+        <v/>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="AO8" t="str">
+      <c r="AO8">
         <f>C8</f>
-        <v>carnegie</v>
+        <v/>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="AO9" t="str">
+      <c r="AO9">
         <f>C9</f>
-        <v>water</v>
+        <v/>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>350</v>
       </c>
       <c r="AO10">
         <f>C10</f>
-        <v>350</v>
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>